<commit_message>
Demo thong Ke voi HashMap
</commit_message>
<xml_diff>
--- a/ManageBookStore/report/SachDB.xlsx
+++ b/ManageBookStore/report/SachDB.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="32">
   <si>
     <t/>
   </si>
@@ -93,6 +93,21 @@
   </si>
   <si>
     <t>KD03.jpg</t>
+  </si>
+  <si>
+    <t>KD04</t>
+  </si>
+  <si>
+    <t>NXB_Đại_Học_Quốc_Gia</t>
+  </si>
+  <si>
+    <t>P.Việt</t>
+  </si>
+  <si>
+    <t>Trường Làng</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -143,14 +158,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="9.5859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="20.7265625" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.2421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.1953125" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="18.02734375" customWidth="true" bestFit="true"/>
     <col min="5" max="5" width="28.71875" customWidth="true" bestFit="true"/>
@@ -276,6 +291,35 @@
         <v>26</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2020.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>125.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>25000.0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>